<commit_message>
flip, ui, basic inventory
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="3980" windowWidth="22300" windowHeight="10700" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="2480" windowWidth="23220" windowHeight="12500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="187">
   <si>
     <t>id</t>
   </si>
@@ -30,24 +30,9 @@
     <t>net neutrality</t>
   </si>
   <si>
-    <t>trump</t>
-  </si>
-  <si>
-    <t>trump hair</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
-    <t>el pollo diablo</t>
-  </si>
-  <si>
-    <t>bitcoin</t>
-  </si>
-  <si>
-    <t>litcoin</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
@@ -105,33 +90,12 @@
     <t>garbage can</t>
   </si>
   <si>
-    <t>generic hat</t>
-  </si>
-  <si>
-    <t>5+6</t>
-  </si>
-  <si>
-    <t>5+7</t>
-  </si>
-  <si>
     <t>big smoke order</t>
   </si>
   <si>
-    <t>15+16</t>
-  </si>
-  <si>
-    <t>shitcoin</t>
-  </si>
-  <si>
-    <t>3+5</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
-    <t>19+19</t>
-  </si>
-  <si>
     <t>visual</t>
   </si>
   <si>
@@ -153,102 +117,15 @@
     <t>generic shirt</t>
   </si>
   <si>
-    <t>beanie</t>
-  </si>
-  <si>
-    <t>battle royale book</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
     <t>recipes</t>
   </si>
   <si>
-    <t>common skin</t>
-  </si>
-  <si>
-    <t>uncommon skin</t>
-  </si>
-  <si>
-    <t>rare skin</t>
-  </si>
-  <si>
-    <t>legendary skin</t>
-  </si>
-  <si>
-    <t>bear skin</t>
-  </si>
-  <si>
-    <t>common knife</t>
-  </si>
-  <si>
-    <t>uncommon knife</t>
-  </si>
-  <si>
-    <t>rare knife</t>
-  </si>
-  <si>
-    <t>legendary knife</t>
-  </si>
-  <si>
-    <t>kitchen knife</t>
-  </si>
-  <si>
-    <t>breakfast</t>
-  </si>
-  <si>
-    <t>new orleans sauteed chicken</t>
-  </si>
-  <si>
-    <t>russia</t>
-  </si>
-  <si>
-    <t>life</t>
-  </si>
-  <si>
-    <t>3 squared</t>
-  </si>
-  <si>
-    <t>108+108</t>
-  </si>
-  <si>
-    <t>109+109</t>
-  </si>
-  <si>
-    <t>110+110</t>
-  </si>
-  <si>
-    <t>107+107</t>
-  </si>
-  <si>
-    <t>111+111</t>
-  </si>
-  <si>
-    <t>112+112</t>
-  </si>
-  <si>
-    <t>113+113</t>
-  </si>
-  <si>
-    <t>114+114</t>
-  </si>
-  <si>
-    <t>115+115</t>
-  </si>
-  <si>
     <t>pay2win medal</t>
   </si>
   <si>
-    <t>finalstand</t>
-  </si>
-  <si>
-    <t>dead man's hand</t>
-  </si>
-  <si>
-    <t>commando pro</t>
-  </si>
-  <si>
     <t>boots on the ground</t>
   </si>
   <si>
@@ -270,15 +147,9 @@
     <t>refined metal</t>
   </si>
   <si>
-    <t>hmm yes quite refined</t>
-  </si>
-  <si>
     <t>what this is made of</t>
   </si>
   <si>
-    <t>fried chicken seasoning</t>
-  </si>
-  <si>
     <t>season pass</t>
   </si>
   <si>
@@ -291,10 +162,424 @@
     <t>There is a review embargo up, but I trust the developers this time.</t>
   </si>
   <si>
-    <t>Starts with a number</t>
-  </si>
-  <si>
-    <t>25+25+25+22+23+27</t>
+    <t>major league chips</t>
+  </si>
+  <si>
+    <t>x2 exp for 2 hours</t>
+  </si>
+  <si>
+    <t>we lost the battle and the war</t>
+  </si>
+  <si>
+    <t>spare change</t>
+  </si>
+  <si>
+    <t>prometheus gift</t>
+  </si>
+  <si>
+    <t>hmm yes quite</t>
+  </si>
+  <si>
+    <t>metal with top hat</t>
+  </si>
+  <si>
+    <t>a pair of socks</t>
+  </si>
+  <si>
+    <t>make recipes, not items</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>iEat</t>
+  </si>
+  <si>
+    <t>I'll have a number 9, a number 9 large…</t>
+  </si>
+  <si>
+    <t>15+15+15</t>
+  </si>
+  <si>
+    <t>finger licking good</t>
+  </si>
+  <si>
+    <t>ice cube</t>
+  </si>
+  <si>
+    <t>nuclear fallout</t>
+  </si>
+  <si>
+    <t>war, war never changes</t>
+  </si>
+  <si>
+    <t>11+17</t>
+  </si>
+  <si>
+    <t>soldier</t>
+  </si>
+  <si>
+    <t>generic shooter</t>
+  </si>
+  <si>
+    <t>nuke</t>
+  </si>
+  <si>
+    <t>deBono</t>
+  </si>
+  <si>
+    <t>I'm a thinker</t>
+  </si>
+  <si>
+    <t>fake money</t>
+  </si>
+  <si>
+    <t>fake smart contract</t>
+  </si>
+  <si>
+    <t>normiecash</t>
+  </si>
+  <si>
+    <t>19+20</t>
+  </si>
+  <si>
+    <t>regulating the deregulated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patrolling the mojave makes you wish for a </t>
+  </si>
+  <si>
+    <t>nuclear winter</t>
+  </si>
+  <si>
+    <t>16+18</t>
+  </si>
+  <si>
+    <t>9+10</t>
+  </si>
+  <si>
+    <t>bad consumer practices</t>
+  </si>
+  <si>
+    <t>I swear the last time I am doing this</t>
+  </si>
+  <si>
+    <t>MLG man</t>
+  </si>
+  <si>
+    <t>major league beverage</t>
+  </si>
+  <si>
+    <t>gulp gulp</t>
+  </si>
+  <si>
+    <t>21+12</t>
+  </si>
+  <si>
+    <t>recursion</t>
+  </si>
+  <si>
+    <t>friend's credit card</t>
+  </si>
+  <si>
+    <t>what they don't know can't hurt them</t>
+  </si>
+  <si>
+    <t>casino chips</t>
+  </si>
+  <si>
+    <t>one you eat, one you don't</t>
+  </si>
+  <si>
+    <t>12+23</t>
+  </si>
+  <si>
+    <t>rich man</t>
+  </si>
+  <si>
+    <t>MLG</t>
+  </si>
+  <si>
+    <t>quarter-lambda 3</t>
+  </si>
+  <si>
+    <t>burger</t>
+  </si>
+  <si>
+    <t>fries</t>
+  </si>
+  <si>
+    <t>value combo</t>
+  </si>
+  <si>
+    <t>24+25</t>
+  </si>
+  <si>
+    <t>that healthy value combo</t>
+  </si>
+  <si>
+    <t>24+14</t>
+  </si>
+  <si>
+    <t>26+16</t>
+  </si>
+  <si>
+    <t>$12 a month for streaming</t>
+  </si>
+  <si>
+    <t>this week he's mopping floors</t>
+  </si>
+  <si>
+    <t>next week it's the fries</t>
+  </si>
+  <si>
+    <t>fidget spinner</t>
+  </si>
+  <si>
+    <t>merge up to 3</t>
+  </si>
+  <si>
+    <t>4+4+4</t>
+  </si>
+  <si>
+    <t>keeping it hip</t>
+  </si>
+  <si>
+    <t>hot new unreleased game</t>
+  </si>
+  <si>
+    <t>watch flicks and chill</t>
+  </si>
+  <si>
+    <t>sun</t>
+  </si>
+  <si>
+    <t>moon</t>
+  </si>
+  <si>
+    <t>mars</t>
+  </si>
+  <si>
+    <t>crab</t>
+  </si>
+  <si>
+    <t>VR headset</t>
+  </si>
+  <si>
+    <t>7+7</t>
+  </si>
+  <si>
+    <t>crowbar</t>
+  </si>
+  <si>
+    <t>gorilla</t>
+  </si>
+  <si>
+    <t>harambe the dead meme (gorilla)</t>
+  </si>
+  <si>
+    <t>34+35</t>
+  </si>
+  <si>
+    <t>32+33+4</t>
+  </si>
+  <si>
+    <t>sniper</t>
+  </si>
+  <si>
+    <t>I paid $60 for dlc, all I got was this t-shirt</t>
+  </si>
+  <si>
+    <t>generic pants</t>
+  </si>
+  <si>
+    <t>fancy knife</t>
+  </si>
+  <si>
+    <t>butter knife</t>
+  </si>
+  <si>
+    <t>revenge is best served cold</t>
+  </si>
+  <si>
+    <t>RNG</t>
+  </si>
+  <si>
+    <t>opening crates and saving the world</t>
+  </si>
+  <si>
+    <t>makes a mean crab patty</t>
+  </si>
+  <si>
+    <t>goodbye internet</t>
+  </si>
+  <si>
+    <t>11+26</t>
+  </si>
+  <si>
+    <t>hello money</t>
+  </si>
+  <si>
+    <t>from the gang called…</t>
+  </si>
+  <si>
+    <t>never know when you need one</t>
+  </si>
+  <si>
+    <t>36+36+36</t>
+  </si>
+  <si>
+    <t>you feel lucky punk</t>
+  </si>
+  <si>
+    <t>spy</t>
+  </si>
+  <si>
+    <t>here to steal your stuff</t>
+  </si>
+  <si>
+    <t>37+32</t>
+  </si>
+  <si>
+    <t>a tf2 classic</t>
+  </si>
+  <si>
+    <t>small cylindrical wealth</t>
+  </si>
+  <si>
+    <t>5+23</t>
+  </si>
+  <si>
+    <t>fakecoin</t>
+  </si>
+  <si>
+    <t>fakecontract</t>
+  </si>
+  <si>
+    <t>future of esports</t>
+  </si>
+  <si>
+    <t>9+21</t>
+  </si>
+  <si>
+    <t>1+33</t>
+  </si>
+  <si>
+    <t>opening gone wrong</t>
+  </si>
+  <si>
+    <t>that's one way to open it</t>
+  </si>
+  <si>
+    <t>8+2</t>
+  </si>
+  <si>
+    <t>inflation ruins trades</t>
+  </si>
+  <si>
+    <t>is this a noun?</t>
+  </si>
+  <si>
+    <t>tops</t>
+  </si>
+  <si>
+    <t>I believe the correct term is beyblade</t>
+  </si>
+  <si>
+    <t>38+27</t>
+  </si>
+  <si>
+    <t>90s person</t>
+  </si>
+  <si>
+    <t>31+38</t>
+  </si>
+  <si>
+    <t>welcome to the future</t>
+  </si>
+  <si>
+    <t>video streaming site</t>
+  </si>
+  <si>
+    <t>fake richness</t>
+  </si>
+  <si>
+    <t>5+19+20</t>
+  </si>
+  <si>
+    <t>a shark tank</t>
+  </si>
+  <si>
+    <t>solar eclipse</t>
+  </si>
+  <si>
+    <t>broken heart</t>
+  </si>
+  <si>
+    <t>baseball bat</t>
+  </si>
+  <si>
+    <t>pencil</t>
+  </si>
+  <si>
+    <t>exploitable webcomic</t>
+  </si>
+  <si>
+    <t>memes</t>
+  </si>
+  <si>
+    <t>44+45</t>
+  </si>
+  <si>
+    <t>love stinks</t>
+  </si>
+  <si>
+    <t>42+3</t>
+  </si>
+  <si>
+    <t>famous painting</t>
+  </si>
+  <si>
+    <t>works of art…somewhat</t>
+  </si>
+  <si>
+    <t>10+40+45</t>
+  </si>
+  <si>
+    <t>corrupted data</t>
+  </si>
+  <si>
+    <t>46+7</t>
+  </si>
+  <si>
+    <t>bugs</t>
+  </si>
+  <si>
+    <t>missingno</t>
+  </si>
+  <si>
+    <t>36+46</t>
+  </si>
+  <si>
+    <t>31+26+20</t>
+  </si>
+  <si>
+    <t>the future of technology</t>
+  </si>
+  <si>
+    <t>tailor tinker</t>
+  </si>
+  <si>
+    <t>37+17</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>aquatic</t>
+  </si>
+  <si>
+    <t>39+32</t>
   </si>
 </sst>
 </file>
@@ -350,8 +635,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -409,7 +716,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -436,6 +743,17 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -462,6 +780,17 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -791,17 +1120,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -809,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -817,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -825,7 +1159,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -833,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -841,21 +1175,29 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="O7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="N8" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -866,13 +1208,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
@@ -881,13 +1223,13 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="N9" t="s">
         <v>0</v>
@@ -896,10 +1238,10 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="Q9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -907,32 +1249,35 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
       </c>
       <c r="G10">
         <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="N10">
-        <f>100</f>
-        <v>100</v>
+        <f>75</f>
+        <v>75</v>
       </c>
       <c r="O10" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="P10" t="s">
+        <v>58</v>
       </c>
       <c r="Q10" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -941,65 +1286,74 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="G11">
         <f>G10+1</f>
         <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="N11">
         <f>N10+1</f>
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="O11" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="P11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <f t="shared" ref="A12:A74" si="0">A11+1</f>
+        <f t="shared" ref="A12:A59" si="0">A11+1</f>
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G35" si="1">G11+1</f>
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ref="G12:G59" si="1">G11+1</f>
-        <v>52</v>
-      </c>
-      <c r="H12" t="s">
-        <v>39</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N34" si="2">N11+1</f>
-        <v>102</v>
+        <f t="shared" ref="N12:N60" si="2">N11+1</f>
+        <v>77</v>
       </c>
       <c r="O12" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="P12" t="s">
+        <v>68</v>
       </c>
       <c r="Q12" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1008,33 +1362,36 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
-        <v>103</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="O13" t="s">
+        <v>72</v>
+      </c>
+      <c r="P13" t="s">
+        <v>74</v>
       </c>
       <c r="Q13" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1043,10 +1400,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
@@ -1057,13 +1417,16 @@
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>104</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>8</v>
+        <v>79</v>
+      </c>
+      <c r="O14" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" t="s">
+        <v>75</v>
       </c>
       <c r="Q14" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1072,24 +1435,33 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
       <c r="J15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="O15" t="s">
-        <v>33</v>
+        <v>80</v>
+      </c>
+      <c r="P15" t="s">
+        <v>79</v>
       </c>
       <c r="Q15" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1098,21 +1470,30 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16">
         <f t="shared" si="2"/>
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="O16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P16" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1121,27 +1502,33 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N17">
         <f t="shared" si="2"/>
-        <v>107</v>
-      </c>
-      <c r="O17">
-        <v>4</v>
+        <v>82</v>
+      </c>
+      <c r="O17" t="s">
+        <v>85</v>
+      </c>
+      <c r="P17" t="s">
+        <v>85</v>
       </c>
       <c r="Q17" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1150,27 +1537,30 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18">
         <f t="shared" si="2"/>
-        <v>108</v>
-      </c>
-      <c r="O18">
-        <v>8</v>
+        <v>83</v>
+      </c>
+      <c r="O18" t="s">
+        <v>91</v>
+      </c>
+      <c r="P18" t="s">
+        <v>89</v>
       </c>
       <c r="Q18" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1179,27 +1569,27 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19">
         <f t="shared" si="2"/>
-        <v>109</v>
-      </c>
-      <c r="O19">
-        <v>16</v>
+        <v>84</v>
+      </c>
+      <c r="P19" t="s">
+        <v>96</v>
       </c>
       <c r="Q19" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1209,26 +1599,29 @@
       </c>
       <c r="B20" t="s">
         <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="J20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20">
         <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="O20">
-        <v>32</v>
+        <v>85</v>
+      </c>
+      <c r="P20" t="s">
+        <v>98</v>
       </c>
       <c r="Q20" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1237,24 +1630,30 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
       <c r="J21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N21">
         <f t="shared" si="2"/>
-        <v>111</v>
-      </c>
-      <c r="O21">
-        <v>64</v>
+        <v>86</v>
+      </c>
+      <c r="P21" t="s">
+        <v>109</v>
       </c>
       <c r="Q21" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1263,24 +1662,33 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>134</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
+      <c r="H22" t="s">
+        <v>30</v>
+      </c>
       <c r="J22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N22">
         <f t="shared" si="2"/>
-        <v>112</v>
-      </c>
-      <c r="O22">
-        <v>128</v>
+        <v>87</v>
+      </c>
+      <c r="O22" t="s">
+        <v>108</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="Q22" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1289,24 +1697,30 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
+      <c r="H23" t="s">
+        <v>34</v>
+      </c>
       <c r="J23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N23">
         <f t="shared" si="2"/>
-        <v>113</v>
-      </c>
-      <c r="O23">
-        <v>256</v>
+        <v>88</v>
+      </c>
+      <c r="P23" t="s">
+        <v>118</v>
       </c>
       <c r="Q23" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1315,24 +1729,27 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
       <c r="J24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N24">
         <f t="shared" si="2"/>
-        <v>114</v>
-      </c>
-      <c r="O24">
-        <v>512</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>69</v>
+        <v>89</v>
+      </c>
+      <c r="P24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1341,24 +1758,33 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>133</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
       <c r="J25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N25">
         <f t="shared" si="2"/>
-        <v>115</v>
-      </c>
-      <c r="O25">
-        <v>1024</v>
+        <v>90</v>
+      </c>
+      <c r="O25" t="s">
+        <v>132</v>
+      </c>
+      <c r="P25" t="s">
+        <v>130</v>
       </c>
       <c r="Q25" t="s">
-        <v>70</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1367,24 +1793,30 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
+      <c r="H26" t="s">
+        <v>123</v>
+      </c>
       <c r="J26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N26">
         <f t="shared" si="2"/>
-        <v>116</v>
-      </c>
-      <c r="O26">
-        <v>2048</v>
+        <v>91</v>
+      </c>
+      <c r="P26" t="s">
+        <v>136</v>
       </c>
       <c r="Q26" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1392,22 +1824,25 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
+      <c r="B27" t="s">
+        <v>67</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N27">
         <f t="shared" si="2"/>
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="P27" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1415,19 +1850,28 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B28">
-        <v>2</v>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N28">
         <f t="shared" si="2"/>
-        <v>118</v>
+        <v>93</v>
+      </c>
+      <c r="P28" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1435,19 +1879,28 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B29">
-        <v>3</v>
+      <c r="B29" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N29">
         <f t="shared" si="2"/>
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="P29" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1455,22 +1908,34 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B30">
-        <v>5</v>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H30" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="J30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N30">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>95</v>
+      </c>
+      <c r="O30" t="s">
+        <v>149</v>
+      </c>
+      <c r="P30" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1478,22 +1943,31 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B31">
-        <v>6</v>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>87</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="J31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N31">
         <f t="shared" si="2"/>
-        <v>121</v>
+        <v>96</v>
+      </c>
+      <c r="P31" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -1501,458 +1975,478 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B32">
-        <v>7</v>
+      <c r="B32" t="s">
+        <v>88</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="H32" t="s">
-        <v>72</v>
-      </c>
       <c r="J32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N32">
         <f t="shared" si="2"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>97</v>
+      </c>
+      <c r="O32" t="s">
+        <v>154</v>
+      </c>
+      <c r="P32" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B33">
-        <v>8</v>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>102</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="H33" t="s">
-        <v>73</v>
-      </c>
       <c r="J33">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N33">
         <f t="shared" si="2"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>98</v>
+      </c>
+      <c r="P33" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B34">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="H34" t="s">
-        <v>74</v>
-      </c>
       <c r="J34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N34">
         <f t="shared" si="2"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>99</v>
+      </c>
+      <c r="P34" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B35">
-        <v>10</v>
+      <c r="B35" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" t="s">
+        <v>101</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="H35" t="s">
-        <v>75</v>
-      </c>
       <c r="J35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>5</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="P35" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="P36" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="P37" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="P38" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="P39" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="P40" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" t="s">
+        <v>129</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="P41" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B42" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="P42" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>117</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" t="s">
+        <v>138</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" t="s">
+        <v>152</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>162</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>172</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>163</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B52" t="s">
+        <v>165</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="G36">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="H36" t="s">
-        <v>76</v>
-      </c>
-      <c r="J36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B37">
-        <v>42</v>
-      </c>
-      <c r="C37" t="s">
-        <v>61</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="J37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="J38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="J39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="G40">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="G41">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="H42" t="s">
-        <v>44</v>
-      </c>
-      <c r="J42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="H43" t="s">
-        <v>45</v>
-      </c>
-      <c r="J43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="J44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="J45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="J46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="J47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="J48">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="J49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="H50" t="s">
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>175</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="J50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="H51" t="s">
+      <c r="N57">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="J51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="N58">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="G53">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="H53" t="s">
-        <v>51</v>
-      </c>
-      <c r="J53">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="G54">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="H54" t="s">
-        <v>52</v>
-      </c>
-      <c r="J54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="G55">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="H55" t="s">
-        <v>53</v>
-      </c>
-      <c r="J55">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="G56">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="H56" t="s">
-        <v>54</v>
-      </c>
-      <c r="J56">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="G57">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="H57" t="s">
-        <v>55</v>
-      </c>
-      <c r="J57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="H58" t="s">
-        <v>56</v>
-      </c>
-      <c r="J58">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="H59" t="s">
-        <v>57</v>
-      </c>
-      <c r="J59">
-        <v>5</v>
+      <c r="N59">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="N60">
+        <f t="shared" si="2"/>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
art up to 50
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-280" yWindow="3320" windowWidth="23220" windowHeight="12500" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="3300" windowWidth="23220" windowHeight="12500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="215">
   <si>
     <t>id</t>
   </si>
@@ -369,9 +370,6 @@
     <t>gorilla</t>
   </si>
   <si>
-    <t>harambe the dead meme (gorilla)</t>
-  </si>
-  <si>
     <t>34+35</t>
   </si>
   <si>
@@ -393,9 +391,6 @@
     <t>butter knife</t>
   </si>
   <si>
-    <t>revenge is best served cold</t>
-  </si>
-  <si>
     <t>RNG</t>
   </si>
   <si>
@@ -462,27 +457,6 @@
     <t>inflation ruins trades</t>
   </si>
   <si>
-    <t>is this a noun?</t>
-  </si>
-  <si>
-    <t>tops</t>
-  </si>
-  <si>
-    <t>I believe the correct term is beyblade</t>
-  </si>
-  <si>
-    <t>38+27</t>
-  </si>
-  <si>
-    <t>90s person</t>
-  </si>
-  <si>
-    <t>31+38</t>
-  </si>
-  <si>
-    <t>welcome to the future</t>
-  </si>
-  <si>
     <t>video streaming site</t>
   </si>
   <si>
@@ -495,39 +469,18 @@
     <t>a shark tank</t>
   </si>
   <si>
-    <t>broken heart</t>
-  </si>
-  <si>
     <t>baseball bat</t>
   </si>
   <si>
     <t>pencil</t>
   </si>
   <si>
-    <t>exploitable webcomic</t>
-  </si>
-  <si>
-    <t>memes</t>
-  </si>
-  <si>
-    <t>44+45</t>
-  </si>
-  <si>
-    <t>love stinks</t>
-  </si>
-  <si>
-    <t>42+3</t>
-  </si>
-  <si>
     <t>famous painting</t>
   </si>
   <si>
     <t>works of art…somewhat</t>
   </si>
   <si>
-    <t>10+40+45</t>
-  </si>
-  <si>
     <t>corrupted data</t>
   </si>
   <si>
@@ -598,6 +551,120 @@
   </si>
   <si>
     <t>up to 100?</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>10+40</t>
+  </si>
+  <si>
+    <t>magnifying glass</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>christmas</t>
+  </si>
+  <si>
+    <t>50+51</t>
+  </si>
+  <si>
+    <t>contemporary art</t>
+  </si>
+  <si>
+    <t>backstab</t>
+  </si>
+  <si>
+    <t>35+37</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>38+6</t>
+  </si>
+  <si>
+    <t>burning ants</t>
+  </si>
+  <si>
+    <t>harambe</t>
+  </si>
+  <si>
+    <t>theme</t>
+  </si>
+  <si>
+    <t>video games</t>
+  </si>
+  <si>
+    <t>dlc</t>
+  </si>
+  <si>
+    <t>useless skin</t>
+  </si>
+  <si>
+    <t>midi soundtrack</t>
+  </si>
+  <si>
+    <t>one time use items</t>
+  </si>
+  <si>
+    <t>beluga card</t>
+  </si>
+  <si>
+    <t>sharks beware</t>
+  </si>
+  <si>
+    <t>un is better than deus</t>
+  </si>
+  <si>
+    <t>sounds good</t>
+  </si>
+  <si>
+    <t>map pack</t>
+  </si>
+  <si>
+    <t>4 multiplayer, 1 zombie</t>
+  </si>
+  <si>
+    <t>orange and blue box</t>
+  </si>
+  <si>
+    <t>expansion pack</t>
+  </si>
+  <si>
+    <t>more civilizations</t>
+  </si>
+  <si>
+    <t>early adopter</t>
+  </si>
+  <si>
+    <t>early investments</t>
+  </si>
+  <si>
+    <t>future games</t>
+  </si>
+  <si>
+    <t>portable</t>
+  </si>
+  <si>
+    <t>merge 2</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>icons</t>
   </si>
 </sst>
 </file>
@@ -636,7 +703,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +713,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,7 +732,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -777,13 +850,55 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -842,6 +957,26 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -900,6 +1035,26 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1229,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1323,7 +1478,7 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
@@ -1365,6 +1520,9 @@
       </c>
       <c r="D10" t="s">
         <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
       </c>
       <c r="G10">
         <v>50</v>
@@ -1403,6 +1561,9 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
       <c r="G11">
         <f>G10+1</f>
         <v>51</v>
@@ -1426,7 +1587,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <f t="shared" ref="A12:A59" si="0">A11+1</f>
+        <f t="shared" ref="A12:A75" si="0">A11+1</f>
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1437,6 +1598,9 @@
       </c>
       <c r="D12" t="s">
         <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12:G35" si="1">G11+1</f>
@@ -1468,13 +1632,16 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
@@ -1514,12 +1681,15 @@
       <c r="D14" t="s">
         <v>50</v>
       </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
       <c r="G14">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1548,6 +1718,9 @@
       </c>
       <c r="D15" t="s">
         <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
@@ -1584,6 +1757,9 @@
       <c r="D16" t="s">
         <v>42</v>
       </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
       <c r="G16">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -1619,6 +1795,9 @@
       <c r="D17" t="s">
         <v>52</v>
       </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
       <c r="G17">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -1651,6 +1830,9 @@
       <c r="D18" t="s">
         <v>44</v>
       </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
       <c r="G18">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -1683,6 +1865,9 @@
       <c r="D19" t="s">
         <v>46</v>
       </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
       <c r="G19">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -1712,12 +1897,15 @@
       <c r="D20" t="s">
         <v>49</v>
       </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
       <c r="G20">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J20">
         <v>3</v>
@@ -1743,6 +1931,9 @@
       </c>
       <c r="D21" t="s">
         <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
@@ -1774,7 +1965,10 @@
         <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
@@ -1797,7 +1991,7 @@
         <v>92</v>
       </c>
       <c r="Q22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1810,6 +2004,9 @@
       </c>
       <c r="D23" t="s">
         <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
@@ -1826,10 +2023,10 @@
         <v>88</v>
       </c>
       <c r="P23" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q23" t="s">
         <v>116</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1842,6 +2039,9 @@
       </c>
       <c r="D24" t="s">
         <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
@@ -1857,9 +2057,6 @@
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
-      <c r="P24" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25">
@@ -1870,7 +2067,10 @@
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
@@ -1886,6 +2086,12 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
+      <c r="P25" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26">
@@ -1897,13 +2103,16 @@
       </c>
       <c r="D26" t="s">
         <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="H26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J26">
         <v>4</v>
@@ -1913,10 +2122,10 @@
         <v>91</v>
       </c>
       <c r="P26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1926,6 +2135,9 @@
       </c>
       <c r="B27" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
@@ -1939,10 +2151,10 @@
         <v>92</v>
       </c>
       <c r="P27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1951,10 +2163,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D28" t="s">
         <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
@@ -1968,10 +2183,10 @@
         <v>93</v>
       </c>
       <c r="P28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1980,10 +2195,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D29" t="s">
         <v>70</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
@@ -1997,10 +2215,10 @@
         <v>94</v>
       </c>
       <c r="P29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2013,13 +2231,16 @@
       </c>
       <c r="D30" t="s">
         <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J30">
         <v>5</v>
@@ -2029,13 +2250,13 @@
         <v>95</v>
       </c>
       <c r="O30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="Q30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2048,13 +2269,16 @@
       </c>
       <c r="D31" t="s">
         <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J31">
         <v>5</v>
@@ -2064,10 +2288,10 @@
         <v>96</v>
       </c>
       <c r="P31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Q31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2077,6 +2301,9 @@
       </c>
       <c r="B32" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
@@ -2089,15 +2316,6 @@
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="O32" t="s">
-        <v>149</v>
-      </c>
-      <c r="P32" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33">
@@ -2109,6 +2327,9 @@
       </c>
       <c r="D33" t="s">
         <v>101</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
@@ -2121,12 +2342,6 @@
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-      <c r="P33" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34">
@@ -2138,6 +2353,9 @@
       </c>
       <c r="D34" t="s">
         <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -2151,10 +2369,10 @@
         <v>99</v>
       </c>
       <c r="P34" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="Q34" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2163,10 +2381,13 @@
         <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D35" t="s">
         <v>100</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
@@ -2179,12 +2400,6 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="P35" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36">
@@ -2197,15 +2412,18 @@
       <c r="D36" t="s">
         <v>106</v>
       </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
       <c r="N36">
         <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="P36" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="Q36" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2216,15 +2434,18 @@
       <c r="B37" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
       <c r="N37">
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="P37" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="Q37" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2235,15 +2456,18 @@
       <c r="B38" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
       <c r="N38">
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="P38" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="Q38" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2252,17 +2476,20 @@
         <v>30</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>180</v>
+        <v>164</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
       </c>
       <c r="N39">
         <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="P39" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="Q39" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -2270,18 +2497,21 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="E40" t="s">
+        <v>193</v>
+      </c>
       <c r="N40">
         <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="P40" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="Q40" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -2289,21 +2519,24 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>125</v>
+      </c>
+      <c r="E41" t="s">
+        <v>193</v>
       </c>
       <c r="N41">
         <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="P41" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="Q41" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -2311,21 +2544,24 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>193</v>
       </c>
       <c r="N42">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="P42" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="Q42" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -2333,18 +2569,21 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="E43" t="s">
+        <v>193</v>
+      </c>
       <c r="N43">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="P43" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="Q43" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -2352,18 +2591,21 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B44" t="s">
-        <v>119</v>
+      <c r="B44" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>193</v>
       </c>
       <c r="N44">
         <f t="shared" si="2"/>
         <v>109</v>
       </c>
       <c r="P44" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="Q44" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -2371,12 +2613,21 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B45" t="s">
-        <v>125</v>
+      <c r="B45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" t="s">
+        <v>193</v>
       </c>
       <c r="N45">
         <f t="shared" si="2"/>
         <v>110</v>
+      </c>
+      <c r="P45" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -2384,11 +2635,14 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B46" t="s">
-        <v>132</v>
+      <c r="B46" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="E46" t="s">
+        <v>193</v>
       </c>
       <c r="N46">
         <f t="shared" si="2"/>
@@ -2400,11 +2654,11 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B47" t="s">
-        <v>151</v>
-      </c>
-      <c r="D47" t="s">
-        <v>147</v>
+      <c r="B47" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E47" t="s">
+        <v>193</v>
       </c>
       <c r="N47">
         <f t="shared" si="2"/>
@@ -2416,8 +2670,11 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B48" t="s">
-        <v>157</v>
+      <c r="B48" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" t="s">
+        <v>193</v>
       </c>
       <c r="N48">
         <f t="shared" si="2"/>
@@ -2429,8 +2686,14 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B49" t="s">
-        <v>166</v>
+      <c r="B49" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E49" t="s">
+        <v>193</v>
+      </c>
+      <c r="I49" t="s">
+        <v>188</v>
       </c>
       <c r="N49">
         <f t="shared" si="2"/>
@@ -2442,8 +2705,11 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B50" t="s">
-        <v>191</v>
+      <c r="B50" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" t="s">
+        <v>193</v>
       </c>
       <c r="N50">
         <f t="shared" si="2"/>
@@ -2455,8 +2721,11 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B51" t="s">
-        <v>158</v>
+      <c r="B51" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E51" t="s">
+        <v>193</v>
       </c>
       <c r="N51">
         <f t="shared" si="2"/>
@@ -2468,8 +2737,11 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B52" t="s">
-        <v>159</v>
+      <c r="B52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" t="s">
+        <v>193</v>
       </c>
       <c r="N52">
         <f t="shared" si="2"/>
@@ -2481,8 +2753,11 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B53" t="s">
-        <v>160</v>
+      <c r="B53" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" t="s">
+        <v>193</v>
       </c>
       <c r="N53">
         <f t="shared" si="2"/>
@@ -2495,7 +2770,10 @@
         <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>177</v>
+      </c>
+      <c r="E54" t="s">
+        <v>193</v>
       </c>
       <c r="N54">
         <f t="shared" si="2"/>
@@ -2508,7 +2786,10 @@
         <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>169</v>
+        <v>153</v>
+      </c>
+      <c r="E55" t="s">
+        <v>193</v>
       </c>
       <c r="N55">
         <f t="shared" si="2"/>
@@ -2521,7 +2802,10 @@
         <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>183</v>
+        <v>167</v>
+      </c>
+      <c r="E56" t="s">
+        <v>193</v>
       </c>
       <c r="N56">
         <f t="shared" si="2"/>
@@ -2534,7 +2818,10 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>172</v>
+      </c>
+      <c r="E57" t="s">
+        <v>193</v>
       </c>
       <c r="N57">
         <f t="shared" si="2"/>
@@ -2547,7 +2834,10 @@
         <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>189</v>
+        <v>173</v>
+      </c>
+      <c r="E58" t="s">
+        <v>193</v>
       </c>
       <c r="N58">
         <f t="shared" si="2"/>
@@ -2560,20 +2850,2123 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" t="s">
+        <v>193</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B60" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" t="s">
+        <v>194</v>
+      </c>
+      <c r="G60" t="s">
+        <v>176</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="E61" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B63" t="s">
+        <v>195</v>
+      </c>
+      <c r="E63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B64" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B65" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B66" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E66" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B67" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" t="s">
+        <v>203</v>
+      </c>
+      <c r="E67" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B68" t="s">
+        <v>205</v>
+      </c>
+      <c r="C68" t="s">
+        <v>206</v>
+      </c>
+      <c r="E68" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="E69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="E71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E72" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="E74" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="E75" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <f t="shared" ref="A76:A112" si="3">A75+1</f>
+        <v>67</v>
+      </c>
+      <c r="E76" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="E77" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="E78" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q109"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="O7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>75</f>
+        <v>75</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11">
+        <f>A10+1</f>
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <f>G10+1</f>
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f>N10+1</f>
+        <v>76</v>
+      </c>
+      <c r="O11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <f t="shared" ref="A12:A75" si="0">A11+1</f>
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G35" si="1">G11+1</f>
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12:N60" si="2">N11+1</f>
+        <v>77</v>
+      </c>
+      <c r="O12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="O13" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="O15" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="O16" t="s">
+        <v>91</v>
+      </c>
+      <c r="P16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="O17" t="s">
+        <v>84</v>
+      </c>
+      <c r="P17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="O18" t="s">
+        <v>90</v>
+      </c>
+      <c r="P18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="P19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>214</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="H20" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="P20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>214</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="P21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="H22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="O22" t="s">
+        <v>107</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>214</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="H23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="P23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>214</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="P25" t="s">
         <v>190</v>
       </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>212</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="P26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="P27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>212</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="P28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>214</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="P29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" t="s">
+        <v>213</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H30" t="s">
+        <v>121</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="O30" t="s">
+        <v>142</v>
+      </c>
+      <c r="P30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" t="s">
+        <v>213</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
+        <v>122</v>
+      </c>
+      <c r="J31">
+        <v>5</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="P31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" t="s">
+        <v>213</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="s">
+        <v>213</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="J33">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>213</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="J34">
+        <v>5</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="P34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" t="s">
+        <v>213</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
+        <v>213</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="P36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" t="s">
+        <v>213</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="P37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" t="s">
+        <v>213</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="P38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" t="s">
+        <v>213</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="P39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" t="s">
+        <v>193</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="P40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" t="s">
+        <v>193</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="P41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>193</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="P42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" t="s">
+        <v>193</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="P43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>193</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="P44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" t="s">
+        <v>193</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="P45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" t="s">
+        <v>193</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E47" t="s">
+        <v>193</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" t="s">
+        <v>193</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E49" t="s">
+        <v>193</v>
+      </c>
+      <c r="I49" t="s">
+        <v>188</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" t="s">
+        <v>193</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E51" t="s">
+        <v>193</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" t="s">
+        <v>193</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" t="s">
+        <v>193</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B54" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" t="s">
+        <v>193</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" t="s">
+        <v>193</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="E56" t="s">
+        <v>193</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>172</v>
+      </c>
+      <c r="E57" t="s">
+        <v>193</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>173</v>
+      </c>
+      <c r="E58" t="s">
+        <v>193</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B59" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" t="s">
+        <v>193</v>
+      </c>
       <c r="N59">
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" t="s">
-        <v>192</v>
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B60" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" t="s">
+        <v>194</v>
+      </c>
+      <c r="G60" t="s">
+        <v>176</v>
       </c>
       <c r="N60">
         <f t="shared" si="2"/>
         <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="E61" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B63" t="s">
+        <v>195</v>
+      </c>
+      <c r="E63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B64" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B65" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B66" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E66" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B67" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" t="s">
+        <v>203</v>
+      </c>
+      <c r="E67" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B68" t="s">
+        <v>205</v>
+      </c>
+      <c r="C68" t="s">
+        <v>206</v>
+      </c>
+      <c r="E68" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="E69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="E71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E72" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="E74" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="E75" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <f t="shared" ref="A76:A109" si="3">A75+1</f>
+        <v>67</v>
+      </c>
+      <c r="E76" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="E77" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="E78" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109">
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>